<commit_message>
updated pcb and test results and graphics
All relevant files up to charge injection journal
</commit_message>
<xml_diff>
--- a/Buffer/Quote Documents/BufferRevD_BOM.xlsx
+++ b/Buffer/Quote Documents/BufferRevD_BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kefer\Documents\GitHub\SSB_ChargeInjection\Buffer\Quote Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98D4D3C-6715-4F67-A2C1-0D8A5DACC31E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE69E189-41DA-4BBA-B58B-AF82DDA3A221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{30CB411B-F414-448E-9E1D-ADFE18ACC317}"/>
   </bookViews>
@@ -289,12 +289,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -309,13 +321,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -673,7 +687,7 @@
   <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -754,7 +768,7 @@
       <c r="I2" t="s">
         <v>36</v>
       </c>
-      <c r="K2" s="2"/>
+      <c r="K2" s="4"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3">
@@ -785,7 +799,7 @@
       <c r="I3" t="s">
         <v>43</v>
       </c>
-      <c r="K3" s="2"/>
+      <c r="K3" s="5"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4">
@@ -816,7 +830,7 @@
       <c r="I4" t="s">
         <v>40</v>
       </c>
-      <c r="K4" s="2"/>
+      <c r="K4" s="4"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5">
@@ -847,7 +861,7 @@
       <c r="I5" t="s">
         <v>47</v>
       </c>
-      <c r="K5" s="2"/>
+      <c r="K5" s="4"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6">
@@ -878,7 +892,7 @@
       <c r="I6" t="s">
         <v>52</v>
       </c>
-      <c r="K6" s="2"/>
+      <c r="K6" s="5"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7">
@@ -909,7 +923,7 @@
       <c r="I7" t="s">
         <v>53</v>
       </c>
-      <c r="K7" s="2"/>
+      <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8">
@@ -940,7 +954,7 @@
       <c r="I8" t="s">
         <v>55</v>
       </c>
-      <c r="K8" s="2"/>
+      <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9">
@@ -971,7 +985,7 @@
       <c r="I9" t="s">
         <v>57</v>
       </c>
-      <c r="K9" s="2"/>
+      <c r="K9" s="4"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10">
@@ -1002,7 +1016,7 @@
       <c r="I10" t="s">
         <v>60</v>
       </c>
-      <c r="K10" s="2"/>
+      <c r="K10" s="4"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11">
@@ -1033,7 +1047,7 @@
       <c r="I11" t="s">
         <v>61</v>
       </c>
-      <c r="K11" s="3"/>
+      <c r="K11" s="5"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12">
@@ -1067,7 +1081,7 @@
       <c r="J12" t="s">
         <v>63</v>
       </c>
-      <c r="K12" s="3"/>
+      <c r="K12" s="5"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13">
@@ -1098,7 +1112,7 @@
       <c r="I13" t="s">
         <v>65</v>
       </c>
-      <c r="K13" s="3"/>
+      <c r="K13" s="4"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14">
@@ -1129,17 +1143,17 @@
       <c r="I14" t="s">
         <v>67</v>
       </c>
-      <c r="K14" s="2"/>
+      <c r="K14" s="4"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>15</v>
       </c>
       <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
         <v>75</v>
-      </c>
-      <c r="C15" t="s">
-        <v>28</v>
       </c>
       <c r="D15" t="s">
         <v>29</v>
@@ -1160,7 +1174,7 @@
       <c r="I15" t="s">
         <v>68</v>
       </c>
-      <c r="K15" s="2"/>
+      <c r="K15" s="4"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16">
@@ -1191,7 +1205,7 @@
       <c r="I16" t="s">
         <v>70</v>
       </c>
-      <c r="K16" s="2"/>
+      <c r="K16" s="5"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="F17">

</xml_diff>